<commit_message>
Added the missing runs
</commit_message>
<xml_diff>
--- a/PIV_Campaign_Processing/Pre_Processing/Wallcuts.xlsx
+++ b/PIV_Campaign_Processing/Pre_Processing/Wallcuts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Documents\GitHub\ratzVKI\PIV_Campaign_Processing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Documents\GitHub\ratzVKI\PIV_Campaign_Processing\Pre_Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA0E2F7-C980-4AA4-ABF6-63486D1D4EA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51991B77-33EE-4F63-92FE-D5A214BACDF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1F51DB6-C2AE-454E-B59C-E825C30F28B0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>Fall</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>R_h4_f1200_1_p15</t>
+  </si>
+  <si>
+    <t>R_h1_f750_1_p10</t>
+  </si>
+  <si>
+    <t>Later</t>
   </si>
 </sst>
 </file>
@@ -537,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293E4F06-2AD7-43BD-A393-B33F2190FC77}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +904,7 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C26" s="1">
         <v>4</v>
@@ -907,26 +913,26 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D27" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C28" s="1">
         <v>5</v>
@@ -940,35 +946,35 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C29" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C30" s="1">
         <v>3</v>
       </c>
       <c r="D30" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C31" s="1">
         <v>3</v>
@@ -977,118 +983,149 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C32" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D32" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E32" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C33" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33" s="1">
         <v>4</v>
       </c>
       <c r="E33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="1">
+        <v>4</v>
+      </c>
+      <c r="D34" s="1">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="1">
+        <v>4</v>
+      </c>
+      <c r="D35" s="1">
+        <v>4</v>
+      </c>
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="1">
+        <v>3</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="1">
+        <v>4</v>
+      </c>
+      <c r="D37" s="1">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="1">
-        <v>3</v>
-      </c>
-      <c r="D34" s="1">
-        <v>4</v>
-      </c>
-      <c r="E34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="1">
-        <v>4</v>
-      </c>
-      <c r="D35" s="1">
-        <v>4</v>
-      </c>
-      <c r="E35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="1">
-        <v>4</v>
-      </c>
-      <c r="D36" s="1">
-        <v>4</v>
-      </c>
-      <c r="E36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="1">
-        <v>3</v>
-      </c>
-      <c r="D37" s="1">
-        <v>3</v>
-      </c>
-      <c r="E37" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C38" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D38" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E38" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C39" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D39" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="1">
+        <v>4</v>
+      </c>
+      <c r="D41" s="1">
+        <v>4</v>
+      </c>
+      <c r="E41" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Processing of the missing final runs
</commit_message>
<xml_diff>
--- a/PIV_Campaign_Processing/Pre_Processing/Wallcuts.xlsx
+++ b/PIV_Campaign_Processing/Pre_Processing/Wallcuts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Documents\GitHub\ratzVKI\PIV_Campaign_Processing\Pre_Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51991B77-33EE-4F63-92FE-D5A214BACDF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAE873A-8B07-447E-BD8E-8D29DE032B3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1F51DB6-C2AE-454E-B59C-E825C30F28B0}"/>
+    <workbookView minimized="1" xWindow="-915" yWindow="345" windowWidth="21750" windowHeight="11385" xr2:uid="{D1F51DB6-C2AE-454E-B59C-E825C30F28B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
   <si>
     <t>Fall</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Excellent</t>
-  </si>
-  <si>
-    <t>nan</t>
   </si>
   <si>
     <t>F_h2_f1000_1_s</t>
@@ -543,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293E4F06-2AD7-43BD-A393-B33F2190FC77}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D40" sqref="B3:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +568,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -649,89 +646,89 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1">
-        <v>4</v>
+        <v>-31</v>
       </c>
       <c r="D10" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1">
-        <v>-31</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -739,32 +736,32 @@
         <v>23</v>
       </c>
       <c r="C14" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1">
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1">
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1">
         <v>4</v>
@@ -773,21 +770,21 @@
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -795,13 +792,13 @@
         <v>27</v>
       </c>
       <c r="C18" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D18" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -809,13 +806,13 @@
         <v>28</v>
       </c>
       <c r="C19" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -823,13 +820,13 @@
         <v>29</v>
       </c>
       <c r="C20" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1">
         <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -837,13 +834,13 @@
         <v>30</v>
       </c>
       <c r="C21" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D21" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -857,7 +854,7 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -865,13 +862,13 @@
         <v>32</v>
       </c>
       <c r="C23" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D23" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -879,18 +876,18 @@
         <v>33</v>
       </c>
       <c r="C24" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C25" s="1">
         <v>4</v>
@@ -899,7 +896,7 @@
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -907,13 +904,13 @@
         <v>36</v>
       </c>
       <c r="C26" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D26" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -935,13 +932,13 @@
         <v>38</v>
       </c>
       <c r="C28" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -952,10 +949,10 @@
         <v>3</v>
       </c>
       <c r="D29" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
@@ -969,7 +966,7 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -977,10 +974,10 @@
         <v>41</v>
       </c>
       <c r="C31" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D31" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E31" t="s">
         <v>14</v>
@@ -991,13 +988,13 @@
         <v>42</v>
       </c>
       <c r="C32" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1">
         <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1005,13 +1002,13 @@
         <v>43</v>
       </c>
       <c r="C33" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D33" s="1">
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1025,7 +1022,7 @@
         <v>4</v>
       </c>
       <c r="E34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1033,13 +1030,13 @@
         <v>45</v>
       </c>
       <c r="C35" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D35" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1047,13 +1044,13 @@
         <v>46</v>
       </c>
       <c r="C36" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D36" s="1">
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1061,35 +1058,35 @@
         <v>47</v>
       </c>
       <c r="C37" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E37" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="C38" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D38" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E38" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>50</v>
-      </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C39" s="1">
         <v>0</v>
@@ -1103,29 +1100,15 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C40" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D40" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E40" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" s="1">
-        <v>4</v>
-      </c>
-      <c r="D41" s="1">
-        <v>4</v>
-      </c>
-      <c r="E41" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>